<commit_message>
Modulos Completos en el Panel principal, base de datos final con informacion , ejemplo de reporte
</commit_message>
<xml_diff>
--- a/documentos/sistema/Sistema Final Hospital-Tec.xlsx
+++ b/documentos/sistema/Sistema Final Hospital-Tec.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AppServ\www\sysitlhospital\documentos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paperez\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7155"/>
   </bookViews>
   <sheets>
     <sheet name="Elaboracion" sheetId="1" r:id="rId1"/>
     <sheet name="Dependencias" sheetId="2" r:id="rId2"/>
     <sheet name="Equipos" sheetId="3" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="76">
   <si>
     <t>agendas</t>
   </si>
@@ -212,6 +213,48 @@
   </si>
   <si>
     <t>Se anexa modulo de datos personales</t>
+  </si>
+  <si>
+    <t>Personas</t>
+  </si>
+  <si>
+    <t>Trabajadores</t>
+  </si>
+  <si>
+    <t>Medicos</t>
+  </si>
+  <si>
+    <t>Choferes</t>
+  </si>
+  <si>
+    <t>Departamentos</t>
+  </si>
+  <si>
+    <t>Puestos</t>
+  </si>
+  <si>
+    <t>Datos laborales</t>
+  </si>
+  <si>
+    <t>Administración del sistema</t>
+  </si>
+  <si>
+    <t>Enfermeros</t>
+  </si>
+  <si>
+    <t>Modulos especiales</t>
+  </si>
+  <si>
+    <t>Catalogos generales</t>
+  </si>
+  <si>
+    <t>Descuentos</t>
+  </si>
+  <si>
+    <t>Agendas</t>
+  </si>
+  <si>
+    <t>Hospitalizados</t>
   </si>
 </sst>
 </file>
@@ -417,7 +460,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -468,6 +511,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -483,6 +529,8 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -763,10 +811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M26"/>
+  <dimension ref="A1:M27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,24 +822,24 @@
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="2" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="7" width="13.85546875" customWidth="1"/>
-    <col min="8" max="8" width="15.42578125" customWidth="1"/>
+    <col min="8" max="8" width="3.28515625" customWidth="1"/>
     <col min="9" max="9" width="6.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C1" s="1">
+      <c r="C1" s="26">
         <v>4</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="26">
         <v>4</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="26">
         <v>5</v>
       </c>
-      <c r="F1" s="1">
+      <c r="F1" s="26">
         <v>5</v>
       </c>
-      <c r="G1" s="1">
+      <c r="G1" s="26">
         <v>1</v>
       </c>
     </row>
@@ -888,13 +936,13 @@
       <c r="B7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="29">
         <v>43789</v>
       </c>
-      <c r="D7" s="29"/>
-      <c r="E7" s="29"/>
-      <c r="F7" s="29"/>
-      <c r="G7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="31"/>
       <c r="K7" s="24"/>
       <c r="L7" s="24"/>
       <c r="M7" s="24"/>
@@ -924,7 +972,9 @@
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
-      <c r="F9" s="8"/>
+      <c r="F9" s="20">
+        <v>43796</v>
+      </c>
       <c r="G9" s="4"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -935,7 +985,9 @@
         <v>11</v>
       </c>
       <c r="C10" s="9"/>
-      <c r="D10" s="8"/>
+      <c r="D10" s="20">
+        <v>43796</v>
+      </c>
       <c r="E10" s="9"/>
       <c r="F10" s="9"/>
       <c r="G10" s="9"/>
@@ -977,7 +1029,9 @@
       <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="8"/>
+      <c r="C13" s="20">
+        <v>43796</v>
+      </c>
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
@@ -1008,7 +1062,9 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="8"/>
+      <c r="F15" s="20">
+        <v>43797</v>
+      </c>
       <c r="G15" s="4"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
@@ -1020,7 +1076,9 @@
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="8"/>
+      <c r="E16" s="20">
+        <v>43796</v>
+      </c>
       <c r="F16" s="9"/>
       <c r="G16" s="9"/>
       <c r="K16" s="24"/>
@@ -1049,7 +1107,9 @@
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="8"/>
+      <c r="E18" s="32">
+        <v>43797</v>
+      </c>
       <c r="F18" s="9"/>
       <c r="G18" s="9"/>
     </row>
@@ -1134,19 +1194,27 @@
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="D25" s="26" t="s">
+      <c r="D25" s="27" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="26" spans="1:13" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
+      <c r="C26" s="28"/>
+      <c r="D26" s="28"/>
       <c r="K26" s="25"/>
       <c r="L26" s="25"/>
       <c r="M26" s="25"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="C27" s="33">
+        <v>43797</v>
+      </c>
+      <c r="D27" s="33">
+        <v>43797</v>
+      </c>
     </row>
   </sheetData>
   <sortState ref="A2:B21">
@@ -1399,7 +1467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -1482,4 +1550,210 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:B30"/>
+  <sheetViews>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>8</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>9</v>
+      </c>
+      <c r="B16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>10</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>11</v>
+      </c>
+      <c r="B18" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>14</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>15</v>
+      </c>
+      <c r="B22" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>16</v>
+      </c>
+      <c r="B23" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>17</v>
+      </c>
+      <c r="B26" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>18</v>
+      </c>
+      <c r="B27" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>19</v>
+      </c>
+      <c r="B28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>21</v>
+      </c>
+      <c r="B30" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A25:B30">
+    <sortCondition ref="B26"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>